<commit_message>
Export to Excel has been added with columns' names. Menus' color has been changed from black to default.
</commit_message>
<xml_diff>
--- a/app/ModelGrid/ToExcelExport.xlsx
+++ b/app/ModelGrid/ToExcelExport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>${qAllVisits.fromdate}</t>
   </si>
@@ -31,6 +31,18 @@
   </si>
   <si>
     <t>Visits</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Paid</t>
   </si>
 </sst>
 </file>
@@ -81,13 +93,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -387,7 +402,7 @@
   <dimension ref="C3:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -396,12 +411,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:6">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="3:6">
       <c r="C5" s="1" t="s">

</xml_diff>